<commit_message>
ML: Migrate Keras custom tutorial to Vitis AI 1.3
</commit_message>
<xml_diff>
--- a/Machine_Learning/Design_Tutorials/04-Keras_GoogleNet_ResNet/files/doc/summary_results.xlsx
+++ b/Machine_Learning/Design_Tutorials/04-Keras_GoogleNet_ResNet/files/doc/summary_results.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DeepLearning\VITIS_AI\VAI-KERAS-CUSTOM-GOOGLENET-RESNET\files\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GHE\VAI-KERAS-CUSTOM-GOOGLENET-RESNET\files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B40BB67-DD08-46F4-915A-FFE57A18F684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="988"/>
+    <workbookView xWindow="3510" yWindow="-16545" windowWidth="21600" windowHeight="8670" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VITISAI1.0" sheetId="2" r:id="rId1"/>
+    <sheet name="VITISAI1.3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>CNN</t>
   </si>
@@ -65,9 +66,6 @@
     <t>Run-time</t>
   </si>
   <si>
-    <t>(fps)</t>
-  </si>
-  <si>
     <t>LeNet</t>
   </si>
   <si>
@@ -95,20 +93,29 @@
     <t>activation_83/Softmax</t>
   </si>
   <si>
+    <t>CIFAR-10</t>
+  </si>
+  <si>
     <t>Dell Precision 5820 Tower Desktop with NVIDIA Quadro P6000 GPU 24 GB memory</t>
   </si>
   <si>
-    <t>CIFAR-10</t>
+    <t>Throughput based on 1 thread only (more the threads higher the fps)</t>
+  </si>
+  <si>
+    <t>(fps) 1 thread</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(fps) max </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -132,6 +139,21 @@
     <font>
       <i/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -385,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -411,9 +433,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,6 +526,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,7 +544,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -612,7 +636,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -624,7 +648,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -641,9 +665,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -671,14 +695,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -706,6 +747,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -857,31 +915,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5546875"/>
-    <col min="2" max="2" width="12.109375" style="1"/>
-    <col min="3" max="3" width="12.33203125" style="1"/>
-    <col min="4" max="4" width="7.5546875" style="1"/>
-    <col min="5" max="5" width="14.88671875" style="1"/>
-    <col min="6" max="6" width="20.33203125" style="1"/>
-    <col min="7" max="7" width="7.5546875" style="1"/>
-    <col min="8" max="8" width="12.5546875" style="1"/>
-    <col min="9" max="9" width="15.109375" style="1"/>
-    <col min="10" max="10" width="9.21875" style="1"/>
-    <col min="11" max="11" width="10.88671875" style="1"/>
-    <col min="12" max="12" width="4.88671875" style="1"/>
-    <col min="13" max="1025" width="8.21875"/>
+    <col min="1" max="1" width="11.33203125"/>
+    <col min="2" max="2" width="11.86328125" style="1"/>
+    <col min="3" max="3" width="12.1328125" style="1"/>
+    <col min="4" max="4" width="7.3984375" style="1"/>
+    <col min="5" max="5" width="14.59765625" style="1"/>
+    <col min="6" max="6" width="20" style="1"/>
+    <col min="7" max="7" width="7.3984375" style="1"/>
+    <col min="8" max="8" width="12.3984375" style="1"/>
+    <col min="9" max="9" width="14.86328125" style="1"/>
+    <col min="10" max="10" width="9.19921875" style="1"/>
+    <col min="11" max="11" width="12.796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.73046875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -909,405 +966,424 @@
       <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
+      <c r="L1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="11"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="B4" s="23">
+        <v>478</v>
+      </c>
+      <c r="C4" s="24">
+        <v>6409510</v>
+      </c>
+      <c r="D4" s="25">
+        <v>5</v>
+      </c>
+      <c r="E4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="24">
-        <v>406</v>
-      </c>
-      <c r="C4" s="25">
+      <c r="F4" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="28">
+        <v>0.92</v>
+      </c>
+      <c r="H4" s="28">
+        <v>0.92</v>
+      </c>
+      <c r="I4" s="28">
+        <v>0.92359999999999998</v>
+      </c>
+      <c r="J4" s="29">
+        <v>0.93</v>
+      </c>
+      <c r="K4" s="30">
+        <v>773</v>
+      </c>
+      <c r="L4" s="30">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="23">
+        <v>804</v>
+      </c>
+      <c r="C5" s="24">
+        <v>2170986</v>
+      </c>
+      <c r="D5" s="25">
+        <v>25</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="28">
+        <v>0.94</v>
+      </c>
+      <c r="H5" s="28">
+        <v>0.94120000000000004</v>
+      </c>
+      <c r="I5" s="31">
+        <v>9468</v>
+      </c>
+      <c r="J5" s="29">
+        <v>0.95</v>
+      </c>
+      <c r="K5" s="30">
+        <v>1563</v>
+      </c>
+      <c r="L5" s="30">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="23">
+        <v>3774</v>
+      </c>
+      <c r="C6" s="24">
+        <v>1656250</v>
+      </c>
+      <c r="D6" s="25">
+        <v>70</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="28">
+        <v>0.93</v>
+      </c>
+      <c r="H6" s="28">
+        <v>0.92320000000000002</v>
+      </c>
+      <c r="I6" s="28">
+        <v>0.92579999999999996</v>
+      </c>
+      <c r="J6" s="29">
+        <v>0.93</v>
+      </c>
+      <c r="K6" s="30">
+        <v>907</v>
+      </c>
+      <c r="L6" s="30">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23">
+        <v>7920</v>
+      </c>
+      <c r="C7" s="24">
+        <v>886102</v>
+      </c>
+      <c r="D7" s="25">
+        <v>100</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="H7" s="28">
+        <v>0.94259999999999999</v>
+      </c>
+      <c r="I7" s="28">
+        <v>0.94479999999999997</v>
+      </c>
+      <c r="J7" s="29">
+        <v>0.95</v>
+      </c>
+      <c r="K7" s="30">
+        <v>499</v>
+      </c>
+      <c r="L7" s="30">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="23">
+        <v>399</v>
+      </c>
+      <c r="C9" s="24">
         <v>6409510</v>
       </c>
-      <c r="D4" s="26">
-        <v>5</v>
-      </c>
-      <c r="E4" s="27" t="s">
+      <c r="D9" s="25">
+        <v>20</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="G9" s="28">
+        <v>0.69</v>
+      </c>
+      <c r="H9" s="28">
+        <v>0.68559999999999999</v>
+      </c>
+      <c r="I9" s="28">
+        <v>0.69220000000000004</v>
+      </c>
+      <c r="J9" s="29">
+        <v>0.69</v>
+      </c>
+      <c r="K9" s="30">
+        <v>773</v>
+      </c>
+      <c r="L9" s="30">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="29">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="H4" s="29">
-        <v>0.92120000000000002</v>
-      </c>
-      <c r="I4" s="29">
-        <v>0.92159999999999997</v>
-      </c>
-      <c r="J4" s="30">
+      <c r="B10" s="23">
+        <v>676</v>
+      </c>
+      <c r="C10" s="24">
+        <v>2170986</v>
+      </c>
+      <c r="D10" s="25">
+        <v>40</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="28">
+        <v>0.84</v>
+      </c>
+      <c r="H10" s="28">
+        <v>0.83919999999999995</v>
+      </c>
+      <c r="I10" s="31">
+        <v>0.84760000000000002</v>
+      </c>
+      <c r="J10" s="29">
+        <v>0.84</v>
+      </c>
+      <c r="K10" s="30">
+        <v>1559</v>
+      </c>
+      <c r="L10" s="30">
+        <v>3838</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="23">
+        <v>3069</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1656250</v>
+      </c>
+      <c r="D11" s="25">
+        <v>70</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0.88</v>
+      </c>
+      <c r="H11" s="28">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0.88680000000000003</v>
+      </c>
+      <c r="J11" s="29">
+        <v>0.88</v>
+      </c>
+      <c r="K11" s="30">
+        <v>907</v>
+      </c>
+      <c r="L11" s="30">
+        <v>2057</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="36">
+        <v>7804</v>
+      </c>
+      <c r="C12" s="37">
+        <v>886102</v>
+      </c>
+      <c r="D12" s="38">
+        <v>100</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="28">
         <v>0.93</v>
       </c>
-      <c r="K4" s="31">
-        <v>1441</v>
-      </c>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="24">
-        <v>723</v>
-      </c>
-      <c r="C5" s="25">
-        <v>2170986</v>
-      </c>
-      <c r="D5" s="26">
-        <v>25</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="29">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="H5" s="29">
-        <v>0.94259999999999999</v>
-      </c>
-      <c r="I5" s="32">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="J5" s="30">
-        <v>0.95</v>
-      </c>
-      <c r="K5" s="31">
-        <v>2884</v>
-      </c>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="24">
-        <v>3267</v>
-      </c>
-      <c r="C6" s="25">
-        <v>1656250</v>
-      </c>
-      <c r="D6" s="26">
-        <v>70</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="29">
+      <c r="H12" s="41">
+        <v>0.93340000000000001</v>
+      </c>
+      <c r="I12" s="41">
+        <v>0.93059999999999998</v>
+      </c>
+      <c r="J12" s="42">
         <v>0.93</v>
       </c>
-      <c r="H6" s="29">
-        <v>0.90739999999999998</v>
-      </c>
-      <c r="I6" s="29">
-        <v>0.91520000000000001</v>
-      </c>
-      <c r="J6" s="30">
-        <v>0.93</v>
-      </c>
-      <c r="K6" s="31">
-        <v>2243</v>
-      </c>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="24">
-        <v>7920</v>
-      </c>
-      <c r="C7" s="25">
-        <v>886102</v>
-      </c>
-      <c r="D7" s="26">
-        <v>100</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="29">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="H7" s="29">
-        <v>0.94199999999999995</v>
-      </c>
-      <c r="I7" s="29">
-        <v>0.93779999999999997</v>
-      </c>
-      <c r="J7" s="30">
-        <v>0.94</v>
-      </c>
-      <c r="K7" s="31">
-        <v>918</v>
-      </c>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="24">
-        <v>339</v>
-      </c>
-      <c r="C9" s="25">
-        <v>6409510</v>
-      </c>
-      <c r="D9" s="26">
-        <v>20</v>
-      </c>
-      <c r="E9" s="27" t="s">
+      <c r="K12" s="43">
+        <v>499</v>
+      </c>
+      <c r="L12" s="30">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+    </row>
+    <row r="15" spans="1:12" s="48" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="29">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="H9" s="29">
-        <v>0.66900000000000004</v>
-      </c>
-      <c r="I9" s="29">
-        <v>0.67659999999999998</v>
-      </c>
-      <c r="J9" s="30">
-        <v>0.67</v>
-      </c>
-      <c r="K9" s="31">
-        <v>1444</v>
-      </c>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="24">
-        <v>601</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2170986</v>
-      </c>
-      <c r="D10" s="26">
-        <v>40</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="29">
-        <v>0.84299999999999997</v>
-      </c>
-      <c r="H10" s="29">
-        <v>0.84319999999999995</v>
-      </c>
-      <c r="I10" s="32">
-        <v>0.85160000000000002</v>
-      </c>
-      <c r="J10" s="30">
-        <v>0.84</v>
-      </c>
-      <c r="K10" s="31">
-        <v>2754</v>
-      </c>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="24">
-        <v>2652</v>
-      </c>
-      <c r="C11" s="25">
-        <v>1656250</v>
-      </c>
-      <c r="D11" s="26">
-        <v>70</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="29">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="H11" s="29">
-        <v>0.88119999999999998</v>
-      </c>
-      <c r="I11" s="29">
-        <v>0.88380000000000003</v>
-      </c>
-      <c r="J11" s="30">
-        <v>0.88</v>
-      </c>
-      <c r="K11" s="31">
-        <v>2148</v>
-      </c>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="37">
-        <v>6551</v>
-      </c>
-      <c r="C12" s="38">
-        <v>886102</v>
-      </c>
-      <c r="D12" s="39">
-        <v>100</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="42">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="H12" s="42">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="I12" s="42">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="J12" s="43">
-        <v>0.93</v>
-      </c>
-      <c r="K12" s="44">
-        <v>893</v>
-      </c>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G16"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G17"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G18"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G19"/>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G20"/>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
       <c r="G21"/>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G22"/>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="47"/>
+    <row r="23" spans="7:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G23" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.91388888888888897" bottom="0.91388888888888897" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>